<commit_message>
Added Test Listener Added a new Test Case for repeated User Regitration
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Testdata.xlsx
+++ b/src/main/resources/testdata/Testdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>TestCase</t>
   </si>
@@ -89,6 +89,26 @@
   </si>
   <si>
     <t>kara@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <t>KaranPrinja</t>
+  </si>
+  <si>
+    <t>Test@12345</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>karanprinja@hotmail.com</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1528,10 +1548,18 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="A6" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>21</v>
+      </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
@@ -1651,6 +1679,7 @@
     <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="ktothep@gmail.com"/>
     <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="ktothep@hotmail.com"/>
     <hyperlink ref="D4" r:id="rId3" location="" tooltip="" display="ktothep@yahoo.com"/>
+    <hyperlink ref="D6" r:id="rId4" location="" tooltip="" display="karanprinja@hotmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>